<commit_message>
Updated the analysis.R by including risk of biases and data for the SoE tables
Major revisions:
1) Including risk of bias assessments in the meta objects for all outcomes
2) Creating a big dataframe with summary data for all outcomes that cna be useful for the SoE tables (this need to be finalized).
To do: To finalize the R markdown afterwards.
</commit_message>
<xml_diff>
--- a/data/LSR3_H_2024-01-22.xlsx
+++ b/data/LSR3_H_2024-01-22.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/LRZ Sync+Share/Projects/GALENOS/3. systematic reviews/taar/4_analysis/final_dataset/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/Documents/GitHub/LSR3_taar1_H/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCDA7AF2-A303-8245-9272-7FEF3012F654}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA813AA-6DB1-A44A-8916-E1F1BF25456C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24460" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24460" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -328,12 +328,6 @@
     <t>adverse_event_n</t>
   </si>
   <si>
-    <t>anticholinertgic_symptom_e</t>
-  </si>
-  <si>
-    <t>anticholinertgic_symptom_n</t>
-  </si>
-  <si>
     <t>anxiety_e</t>
   </si>
   <si>
@@ -767,6 +761,12 @@
   </si>
   <si>
     <t>ulotaront 25mg</t>
+  </si>
+  <si>
+    <t>anticholinergic_symptom_e</t>
+  </si>
+  <si>
+    <t>anticholinergic_symptom_n</t>
   </si>
 </sst>
 </file>
@@ -790,7 +790,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -815,6 +815,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -828,7 +834,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -838,6 +844,9 @@
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1144,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DY26"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="CV15" sqref="CV15"/>
+    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
+      <selection activeCell="CS10" sqref="CS10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1450,133 +1459,133 @@
       <c r="CT1" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="CU1" s="1" t="s">
+      <c r="CU1" s="7" t="s">
+        <v>243</v>
+      </c>
+      <c r="CV1" s="7" t="s">
+        <v>244</v>
+      </c>
+      <c r="CW1" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="CV1" s="1" t="s">
+      <c r="CX1" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="CW1" s="1" t="s">
+      <c r="CY1" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="CX1" s="1" t="s">
+      <c r="CZ1" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="CY1" s="1" t="s">
+      <c r="DA1" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="CZ1" s="1" t="s">
+      <c r="DB1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="DA1" s="1" t="s">
+      <c r="DC1" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="DB1" s="1" t="s">
+      <c r="DD1" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="DC1" s="1" t="s">
+      <c r="DE1" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="DD1" s="1" t="s">
+      <c r="DF1" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="DE1" s="1" t="s">
+      <c r="DG1" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="DF1" s="1" t="s">
+      <c r="DH1" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="DG1" s="1" t="s">
+      <c r="DI1" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="DH1" s="1" t="s">
+      <c r="DJ1" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="DI1" s="1" t="s">
+      <c r="DK1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="DJ1" s="1" t="s">
+      <c r="DL1" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="DK1" s="1" t="s">
+      <c r="DM1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="DL1" s="1" t="s">
+      <c r="DN1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="DM1" s="1" t="s">
+      <c r="DO1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="DN1" s="1" t="s">
+      <c r="DP1" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="DO1" s="1" t="s">
+      <c r="DQ1" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="DP1" s="1" t="s">
+      <c r="DR1" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="DQ1" s="1" t="s">
+      <c r="DS1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="DR1" s="1" t="s">
+      <c r="DT1" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="DS1" s="1" t="s">
+      <c r="DU1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="DT1" s="1" t="s">
+      <c r="DV1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="DU1" s="1" t="s">
+      <c r="DW1" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="DV1" s="1" t="s">
+      <c r="DX1" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="DW1" s="1" t="s">
+      <c r="DY1" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="DX1" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="DY1" s="1" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="2" spans="1:129" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C2">
         <v>1</v>
       </c>
       <c r="D2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E2" t="s">
+        <v>127</v>
+      </c>
+      <c r="F2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" t="s">
         <v>147</v>
       </c>
-      <c r="E2" t="s">
-        <v>129</v>
-      </c>
-      <c r="F2" t="s">
+      <c r="H2" t="s">
         <v>148</v>
       </c>
-      <c r="G2" t="s">
+      <c r="I2" t="s">
         <v>149</v>
-      </c>
-      <c r="H2" t="s">
-        <v>150</v>
-      </c>
-      <c r="I2" t="s">
-        <v>151</v>
       </c>
       <c r="J2">
         <v>25</v>
       </c>
       <c r="K2" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L2">
         <v>4</v>
@@ -1585,55 +1594,55 @@
         <v>6</v>
       </c>
       <c r="N2" t="s">
+        <v>151</v>
+      </c>
+      <c r="O2" t="s">
+        <v>152</v>
+      </c>
+      <c r="R2" t="s">
         <v>153</v>
       </c>
-      <c r="O2" t="s">
+      <c r="S2" t="s">
+        <v>142</v>
+      </c>
+      <c r="T2" t="s">
         <v>154</v>
       </c>
-      <c r="R2" t="s">
+      <c r="U2" t="s">
+        <v>142</v>
+      </c>
+      <c r="V2" t="s">
+        <v>129</v>
+      </c>
+      <c r="W2" t="s">
+        <v>142</v>
+      </c>
+      <c r="X2" t="s">
         <v>155</v>
       </c>
-      <c r="S2" t="s">
-        <v>144</v>
-      </c>
-      <c r="T2" t="s">
-        <v>156</v>
-      </c>
-      <c r="U2" t="s">
-        <v>144</v>
-      </c>
-      <c r="V2" t="s">
-        <v>131</v>
-      </c>
-      <c r="W2" t="s">
-        <v>144</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
+        <v>142</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB2" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" t="s">
-        <v>144</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF2" t="s">
         <v>159</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>158</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>159</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>161</v>
       </c>
       <c r="AG2">
         <v>23</v>
@@ -1645,16 +1654,16 @@
         <v>20.12</v>
       </c>
       <c r="AK2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AM2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AN2" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AO2">
         <v>24</v>
@@ -1669,16 +1678,16 @@
         <v>7.94</v>
       </c>
       <c r="AS2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AT2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AU2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BL2" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="BM2">
         <v>23</v>
@@ -1693,13 +1702,13 @@
         <v>2.2000000000000002</v>
       </c>
       <c r="BQ2" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BR2" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BS2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CS2">
         <v>18</v>
@@ -1732,48 +1741,48 @@
         <v>25</v>
       </c>
       <c r="DW2" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX2" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY2" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="3" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" t="s">
+        <v>163</v>
+      </c>
+      <c r="F3" t="s">
+        <v>129</v>
+      </c>
+      <c r="G3" t="s">
         <v>147</v>
       </c>
-      <c r="E3" t="s">
-        <v>165</v>
-      </c>
-      <c r="F3" t="s">
-        <v>131</v>
-      </c>
-      <c r="G3" t="s">
+      <c r="H3" t="s">
+        <v>148</v>
+      </c>
+      <c r="I3" t="s">
         <v>149</v>
-      </c>
-      <c r="H3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I3" t="s">
-        <v>151</v>
       </c>
       <c r="J3">
         <v>14</v>
       </c>
       <c r="K3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="L3">
         <v>1</v>
@@ -1782,55 +1791,55 @@
         <v>6</v>
       </c>
       <c r="N3" t="s">
+        <v>164</v>
+      </c>
+      <c r="O3" t="s">
+        <v>143</v>
+      </c>
+      <c r="R3" t="s">
+        <v>164</v>
+      </c>
+      <c r="S3" t="s">
+        <v>165</v>
+      </c>
+      <c r="T3" t="s">
         <v>166</v>
       </c>
-      <c r="O3" t="s">
-        <v>145</v>
-      </c>
-      <c r="R3" t="s">
-        <v>166</v>
-      </c>
-      <c r="S3" t="s">
-        <v>167</v>
-      </c>
-      <c r="T3" t="s">
-        <v>168</v>
-      </c>
       <c r="U3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="V3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="X3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y3" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="Z3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AA3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AB3" t="s">
+        <v>157</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AD3" t="s">
+        <v>156</v>
+      </c>
+      <c r="AE3" t="s">
+        <v>157</v>
+      </c>
+      <c r="AF3" t="s">
         <v>159</v>
-      </c>
-      <c r="AC3" t="s">
-        <v>158</v>
-      </c>
-      <c r="AD3" t="s">
-        <v>158</v>
-      </c>
-      <c r="AE3" t="s">
-        <v>159</v>
-      </c>
-      <c r="AF3" t="s">
-        <v>161</v>
       </c>
       <c r="AG3">
         <v>14</v>
@@ -1842,16 +1851,16 @@
         <v>19.57</v>
       </c>
       <c r="AK3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AM3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AN3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="AO3">
         <v>14</v>
@@ -1866,16 +1875,16 @@
         <v>7.71</v>
       </c>
       <c r="AS3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AT3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AU3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BL3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="BM3">
         <v>14</v>
@@ -1890,13 +1899,13 @@
         <v>1.99</v>
       </c>
       <c r="BQ3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BR3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BS3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CS3">
         <v>12</v>
@@ -1947,48 +1956,48 @@
         <v>14</v>
       </c>
       <c r="DW3" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX3" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B4" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E4" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="G4" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J4">
         <v>120</v>
       </c>
       <c r="K4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L4">
         <v>43</v>
@@ -1997,55 +2006,55 @@
         <v>4</v>
       </c>
       <c r="N4" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="O4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="R4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="S4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="T4" t="s">
+        <v>153</v>
+      </c>
+      <c r="U4" t="s">
+        <v>171</v>
+      </c>
+      <c r="V4" t="s">
+        <v>166</v>
+      </c>
+      <c r="W4" t="s">
+        <v>171</v>
+      </c>
+      <c r="X4" t="s">
         <v>155</v>
       </c>
-      <c r="U4" t="s">
-        <v>173</v>
-      </c>
-      <c r="V4" t="s">
-        <v>168</v>
-      </c>
-      <c r="W4" t="s">
-        <v>173</v>
-      </c>
-      <c r="X4" t="s">
-        <v>157</v>
-      </c>
       <c r="Y4" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="Z4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA4" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB4" t="s">
         <v>158</v>
       </c>
-      <c r="AA4" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB4" t="s">
-        <v>160</v>
-      </c>
       <c r="AC4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD4" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE4" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF4" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG4">
         <v>120</v>
@@ -2060,16 +2069,16 @@
         <v>18.63</v>
       </c>
       <c r="AK4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL4" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN4" t="s">
         <v>134</v>
-      </c>
-      <c r="AM4" t="s">
-        <v>135</v>
-      </c>
-      <c r="AN4" t="s">
-        <v>136</v>
       </c>
       <c r="AO4">
         <v>120</v>
@@ -2084,16 +2093,16 @@
         <v>5.48</v>
       </c>
       <c r="AS4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AT4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AU4" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV4" t="s">
         <v>135</v>
-      </c>
-      <c r="AV4" t="s">
-        <v>137</v>
       </c>
       <c r="AW4">
         <v>120</v>
@@ -2108,16 +2117,16 @@
         <v>4.38</v>
       </c>
       <c r="BA4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BB4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BC4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BT4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BU4">
         <v>120</v>
@@ -2132,16 +2141,16 @@
         <v>6.57</v>
       </c>
       <c r="BY4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BZ4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="CA4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CB4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="CC4">
         <v>120</v>
@@ -2156,19 +2165,19 @@
         <v>1.9</v>
       </c>
       <c r="CG4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="CH4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="CI4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CJ4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="CK4" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="CL4">
         <v>114</v>
@@ -2180,13 +2189,13 @@
         <v>28</v>
       </c>
       <c r="CP4" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="CQ4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CR4" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="CS4">
         <v>55</v>
@@ -2255,48 +2264,48 @@
         <v>120</v>
       </c>
       <c r="DW4" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY4" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="5" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C5">
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F5" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G5" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I5" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="J5">
         <v>125</v>
       </c>
       <c r="K5" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="L5">
         <v>46</v>
@@ -2305,55 +2314,55 @@
         <v>4</v>
       </c>
       <c r="N5" t="s">
+        <v>174</v>
+      </c>
+      <c r="O5" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="R5" t="s">
+        <v>172</v>
+      </c>
+      <c r="S5" t="s">
+        <v>175</v>
+      </c>
+      <c r="T5" t="s">
         <v>176</v>
       </c>
-      <c r="O5" s="4" t="s">
+      <c r="U5" t="s">
+        <v>175</v>
+      </c>
+      <c r="V5" t="s">
+        <v>129</v>
+      </c>
+      <c r="W5" t="s">
+        <v>175</v>
+      </c>
+      <c r="X5" t="s">
         <v>177</v>
       </c>
-      <c r="R5" t="s">
-        <v>174</v>
-      </c>
-      <c r="S5" t="s">
-        <v>177</v>
-      </c>
-      <c r="T5" t="s">
-        <v>178</v>
-      </c>
-      <c r="U5" t="s">
-        <v>177</v>
-      </c>
-      <c r="V5" t="s">
-        <v>131</v>
-      </c>
-      <c r="W5" t="s">
-        <v>177</v>
-      </c>
-      <c r="X5" t="s">
-        <v>179</v>
-      </c>
       <c r="Y5" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="Z5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB5" t="s">
         <v>158</v>
       </c>
-      <c r="AA5" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB5" t="s">
-        <v>160</v>
-      </c>
       <c r="AC5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD5" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF5" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG5">
         <v>125</v>
@@ -2368,16 +2377,16 @@
         <v>17.89</v>
       </c>
       <c r="AK5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL5" t="s">
+        <v>132</v>
+      </c>
+      <c r="AM5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AN5" t="s">
         <v>134</v>
-      </c>
-      <c r="AM5" t="s">
-        <v>135</v>
-      </c>
-      <c r="AN5" t="s">
-        <v>136</v>
       </c>
       <c r="AO5">
         <v>125</v>
@@ -2392,16 +2401,16 @@
         <v>5.59</v>
       </c>
       <c r="AS5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AT5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AU5" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV5" t="s">
         <v>135</v>
-      </c>
-      <c r="AV5" t="s">
-        <v>137</v>
       </c>
       <c r="AW5">
         <v>125</v>
@@ -2416,16 +2425,16 @@
         <v>4.47</v>
       </c>
       <c r="BA5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BB5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="BC5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BT5" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="BU5">
         <v>125</v>
@@ -2440,16 +2449,16 @@
         <v>6.71</v>
       </c>
       <c r="BY5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="BZ5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="CA5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CB5" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="CC5">
         <v>125</v>
@@ -2464,19 +2473,19 @@
         <v>2.2999999999999998</v>
       </c>
       <c r="CG5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="CH5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="CI5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CJ5" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="CK5" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="CL5">
         <v>113</v>
@@ -2488,13 +2497,13 @@
         <v>28</v>
       </c>
       <c r="CP5" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="CQ5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CR5" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="CS5">
         <v>63</v>
@@ -2563,39 +2572,39 @@
         <v>125</v>
       </c>
       <c r="DW5" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX5" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY5" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="B6" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F6" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H6" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I6" s="2">
         <v>435</v>
@@ -2604,7 +2613,7 @@
         <v>144</v>
       </c>
       <c r="K6" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M6">
         <v>6</v>
@@ -2622,25 +2631,25 @@
         <v>144</v>
       </c>
       <c r="Z6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA6" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB6" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AA6" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB6" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="AC6" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG6" s="2">
         <v>142</v>
@@ -2655,48 +2664,48 @@
         <v>19.07</v>
       </c>
       <c r="AK6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AM6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="DW6" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX6" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="7" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B7" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E7" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F7" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G7" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H7" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I7" s="2">
         <v>435</v>
@@ -2705,7 +2714,7 @@
         <v>145</v>
       </c>
       <c r="K7" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M7">
         <v>6</v>
@@ -2723,25 +2732,25 @@
         <v>145</v>
       </c>
       <c r="Z7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA7" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB7" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AA7" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB7" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="AC7" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF7" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG7" s="2">
         <v>145</v>
@@ -2756,57 +2765,57 @@
         <v>19.27</v>
       </c>
       <c r="AK7" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL7" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AM7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="DW7" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX7" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY7" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="8" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B8" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C8">
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G8" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H8" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I8" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="J8" s="3">
         <v>146</v>
       </c>
       <c r="K8" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M8">
         <v>6</v>
@@ -2824,25 +2833,25 @@
         <v>146</v>
       </c>
       <c r="Z8" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA8" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB8" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AA8" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB8" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="AC8" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE8" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG8">
         <v>145</v>
@@ -2857,57 +2866,57 @@
         <v>18.059999999999999</v>
       </c>
       <c r="AK8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL8" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AM8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="DW8" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX8" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY8" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B9" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C9">
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E9" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F9" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="G9" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H9" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I9" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J9" s="2">
         <v>155</v>
       </c>
       <c r="K9" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M9">
         <v>6</v>
@@ -2925,25 +2934,25 @@
         <v>155</v>
       </c>
       <c r="Z9" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA9" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB9" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AA9" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB9" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="AC9" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF9" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG9" s="2">
         <v>153</v>
@@ -2958,57 +2967,57 @@
         <v>18.55</v>
       </c>
       <c r="AK9" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL9" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AM9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="DW9" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX9" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY9" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="10" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B10" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E10" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F10" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G10" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H10" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I10" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J10" s="2">
         <v>154</v>
       </c>
       <c r="K10" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M10">
         <v>6</v>
@@ -3026,25 +3035,25 @@
         <v>154</v>
       </c>
       <c r="Z10" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA10" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB10" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AA10" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB10" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="AC10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF10" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG10" s="2">
         <v>152</v>
@@ -3059,57 +3068,57 @@
         <v>18.489999999999998</v>
       </c>
       <c r="AK10" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL10" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AM10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="DW10" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX10" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY10" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B11" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F11" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G11" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H11" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I11" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="J11" s="2">
         <v>155</v>
       </c>
       <c r="K11" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="M11">
         <v>6</v>
@@ -3127,25 +3136,25 @@
         <v>155</v>
       </c>
       <c r="Z11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA11" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB11" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="AA11" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB11" s="2" t="s">
-        <v>160</v>
-      </c>
       <c r="AC11" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF11" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG11" s="2">
         <v>155</v>
@@ -3160,57 +3169,57 @@
         <v>18.670000000000002</v>
       </c>
       <c r="AK11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="AL11" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="AM11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="DW11" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX11" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY11" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="12" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B12" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H12" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I12" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J12">
         <v>73</v>
       </c>
       <c r="K12" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L12">
         <v>19</v>
@@ -3219,55 +3228,55 @@
         <v>4</v>
       </c>
       <c r="N12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O12" t="s">
+        <v>196</v>
+      </c>
+      <c r="R12" t="s">
+        <v>197</v>
+      </c>
+      <c r="S12" t="s">
         <v>198</v>
       </c>
-      <c r="R12" t="s">
-        <v>199</v>
-      </c>
-      <c r="S12" t="s">
-        <v>200</v>
-      </c>
       <c r="T12" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="U12" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="V12" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="X12" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Y12" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="Z12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA12" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB12" t="s">
         <v>158</v>
       </c>
-      <c r="AA12" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB12" t="s">
-        <v>160</v>
-      </c>
       <c r="AC12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF12" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG12">
         <v>54</v>
@@ -3282,16 +3291,16 @@
         <v>20.18</v>
       </c>
       <c r="AK12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AL12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AM12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AN12" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AO12">
         <v>54</v>
@@ -3306,16 +3315,16 @@
         <v>6.64</v>
       </c>
       <c r="AS12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AT12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU12" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV12" t="s">
         <v>135</v>
-      </c>
-      <c r="AU12" t="s">
-        <v>135</v>
-      </c>
-      <c r="AV12" t="s">
-        <v>137</v>
       </c>
       <c r="AW12">
         <v>54</v>
@@ -3330,16 +3339,16 @@
         <v>5.81</v>
       </c>
       <c r="BA12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BB12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BC12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BT12" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BU12">
         <v>54</v>
@@ -3354,13 +3363,13 @@
         <v>4.03</v>
       </c>
       <c r="BY12" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BZ12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CA12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CS12">
         <v>23</v>
@@ -3405,48 +3414,48 @@
         <v>72</v>
       </c>
       <c r="DW12" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX12" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY12" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="B13" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C13">
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E13" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F13" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="G13" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H13" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I13" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J13">
         <v>71</v>
       </c>
       <c r="K13" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L13">
         <v>19</v>
@@ -3455,55 +3464,55 @@
         <v>4</v>
       </c>
       <c r="N13" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="O13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="R13" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="S13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="T13" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="U13" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="V13" s="5">
         <v>0</v>
       </c>
       <c r="W13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="X13" s="5">
         <v>2</v>
       </c>
       <c r="Y13" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="Z13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA13" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB13" t="s">
         <v>158</v>
       </c>
-      <c r="AA13" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB13" t="s">
-        <v>160</v>
-      </c>
       <c r="AC13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD13" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG13">
         <v>49</v>
@@ -3518,16 +3527,16 @@
         <v>17.03</v>
       </c>
       <c r="AK13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AL13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AM13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AN13" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AO13">
         <v>49</v>
@@ -3542,16 +3551,16 @@
         <v>6.14</v>
       </c>
       <c r="AS13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AT13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU13" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV13" t="s">
         <v>135</v>
-      </c>
-      <c r="AU13" t="s">
-        <v>135</v>
-      </c>
-      <c r="AV13" t="s">
-        <v>137</v>
       </c>
       <c r="AW13">
         <v>49</v>
@@ -3566,16 +3575,16 @@
         <v>5.85</v>
       </c>
       <c r="BA13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BB13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BC13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BT13" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BU13">
         <v>49</v>
@@ -3590,13 +3599,13 @@
         <v>4.1500000000000004</v>
       </c>
       <c r="BY13" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BZ13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CA13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CS13">
         <v>14</v>
@@ -3641,48 +3650,48 @@
         <v>65</v>
       </c>
       <c r="DW13" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX13" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY13" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="14" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B14" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C14">
         <v>1</v>
       </c>
       <c r="D14" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E14" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="F14" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G14" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H14" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I14" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J14">
         <v>69</v>
       </c>
       <c r="K14" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L14">
         <v>15</v>
@@ -3691,55 +3700,55 @@
         <v>4</v>
       </c>
       <c r="N14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="O14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="R14" t="s">
+        <v>152</v>
+      </c>
+      <c r="S14" t="s">
+        <v>209</v>
+      </c>
+      <c r="T14" t="s">
         <v>154</v>
       </c>
-      <c r="S14" t="s">
-        <v>211</v>
-      </c>
-      <c r="T14" t="s">
-        <v>156</v>
-      </c>
       <c r="U14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="V14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="X14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Y14" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="Z14" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA14" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB14" t="s">
         <v>158</v>
       </c>
-      <c r="AA14" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB14" t="s">
-        <v>160</v>
-      </c>
       <c r="AC14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD14" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE14" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF14" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG14">
         <v>51</v>
@@ -3754,16 +3763,16 @@
         <v>17.670000000000002</v>
       </c>
       <c r="AK14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AL14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AM14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AN14" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AO14">
         <v>51</v>
@@ -3778,16 +3787,16 @@
         <v>6.5</v>
       </c>
       <c r="AS14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AT14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU14" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV14" t="s">
         <v>135</v>
-      </c>
-      <c r="AU14" t="s">
-        <v>135</v>
-      </c>
-      <c r="AV14" t="s">
-        <v>137</v>
       </c>
       <c r="AW14">
         <v>51</v>
@@ -3802,16 +3811,16 @@
         <v>5.41</v>
       </c>
       <c r="BA14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BB14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BC14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BT14" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BU14">
         <v>51</v>
@@ -3826,13 +3835,13 @@
         <v>4.08</v>
       </c>
       <c r="BY14" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BZ14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CA14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CS14">
         <v>23</v>
@@ -3877,48 +3886,48 @@
         <v>68</v>
       </c>
       <c r="DW14" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX14" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY14" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B15" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C15">
         <v>1</v>
       </c>
       <c r="D15" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E15" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="F15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="G15" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H15" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="I15" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="J15">
         <v>74</v>
       </c>
       <c r="K15" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="L15">
         <v>18</v>
@@ -3927,55 +3936,55 @@
         <v>4</v>
       </c>
       <c r="N15" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="O15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="R15" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="S15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="T15" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U15" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="V15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="X15" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="Z15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AA15" t="s">
+        <v>156</v>
+      </c>
+      <c r="AB15" t="s">
         <v>158</v>
       </c>
-      <c r="AA15" t="s">
-        <v>158</v>
-      </c>
-      <c r="AB15" t="s">
-        <v>160</v>
-      </c>
       <c r="AC15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AD15" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="AF15" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="AG15">
         <v>56</v>
@@ -3990,16 +3999,16 @@
         <v>15.78</v>
       </c>
       <c r="AK15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AL15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AM15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="AN15" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="AO15">
         <v>56</v>
@@ -4014,16 +4023,16 @@
         <v>5.1100000000000003</v>
       </c>
       <c r="AS15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="AT15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AU15" t="s">
+        <v>133</v>
+      </c>
+      <c r="AV15" t="s">
         <v>135</v>
-      </c>
-      <c r="AU15" t="s">
-        <v>135</v>
-      </c>
-      <c r="AV15" t="s">
-        <v>137</v>
       </c>
       <c r="AW15">
         <v>56</v>
@@ -4038,16 +4047,16 @@
         <v>5.13</v>
       </c>
       <c r="BA15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BB15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BC15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="BT15" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="BU15">
         <v>56</v>
@@ -4062,13 +4071,13 @@
         <v>4.09</v>
       </c>
       <c r="BY15" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="BZ15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CA15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="CS15">
         <v>36</v>
@@ -4113,45 +4122,45 @@
         <v>71</v>
       </c>
       <c r="DW15" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="DX15" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="DY15" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="16" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B16" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C16">
         <v>1</v>
       </c>
       <c r="D16" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G16" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I16" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J16">
         <v>34</v>
       </c>
       <c r="K16" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="L16">
         <v>18</v>
@@ -4160,28 +4169,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R16" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="T16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="V16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="X16" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y16" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="CS16">
         <v>16</v>
@@ -4226,45 +4235,45 @@
         <v>34</v>
       </c>
       <c r="DW16" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX16" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="17" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="B17" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C17">
         <v>1</v>
       </c>
       <c r="D17" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E17" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F17" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G17" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I17" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J17">
         <v>35</v>
       </c>
       <c r="K17" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="L17">
         <v>14</v>
@@ -4273,28 +4282,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R17" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="S17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="T17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="V17" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="X17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Y17" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="CS17">
         <v>34</v>
@@ -4339,45 +4348,45 @@
         <v>35</v>
       </c>
       <c r="DW17" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX17" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY17" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="B18" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C18">
         <v>1</v>
       </c>
       <c r="D18" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="E18" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="F18" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
       <c r="G18" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I18" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="J18">
         <v>36</v>
       </c>
       <c r="K18" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="L18">
         <v>13</v>
@@ -4386,28 +4395,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R18" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="S18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="T18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="V18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="X18" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y18" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="CS18">
         <v>15</v>
@@ -4452,48 +4461,48 @@
         <v>36</v>
       </c>
       <c r="DW18" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="DX18" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY18" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="19" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B19" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C19">
         <v>1</v>
       </c>
       <c r="D19" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G19" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H19" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I19" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J19">
         <v>68</v>
       </c>
       <c r="K19" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L19">
         <v>15</v>
@@ -4502,22 +4511,22 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="T19" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="U19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="V19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="X19" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y19" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="CS19">
         <v>2</v>
@@ -4544,48 +4553,48 @@
         <v>59</v>
       </c>
       <c r="DW19" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX19" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY19" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="B20" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C20">
         <v>1</v>
       </c>
       <c r="D20" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F20" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="G20" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H20" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="I20" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="J20">
         <v>68</v>
       </c>
       <c r="K20" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="L20">
         <v>15</v>
@@ -4594,28 +4603,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="S20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="T20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="V20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="X20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="Y20" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="CS20">
         <v>32</v>
@@ -4648,45 +4657,45 @@
         <v>62</v>
       </c>
       <c r="DW20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX20" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B21" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C21">
         <v>1</v>
       </c>
       <c r="D21" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E21" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F21" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G21" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I21" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J21">
         <v>12</v>
       </c>
       <c r="K21" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L21">
         <v>0</v>
@@ -4695,28 +4704,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="S21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="V21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="X21" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y21" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="CS21">
         <v>1</v>
@@ -4749,45 +4758,45 @@
         <v>12</v>
       </c>
       <c r="DW21" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX21" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B22" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C22">
         <v>1</v>
       </c>
       <c r="D22" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F22" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G22" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I22" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J22">
         <v>12</v>
       </c>
       <c r="K22" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L22">
         <v>0</v>
@@ -4796,28 +4805,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="S22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="T22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="V22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="X22" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y22" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="CS22">
         <v>1</v>
@@ -4850,45 +4859,45 @@
         <v>12</v>
       </c>
       <c r="DW22" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX22" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY22" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="23" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B23" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C23">
         <v>1</v>
       </c>
       <c r="D23" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G23" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="I23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="J23">
         <v>24</v>
       </c>
       <c r="K23" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="L23">
         <v>0</v>
@@ -4897,28 +4906,28 @@
         <v>0.14000000000000001</v>
       </c>
       <c r="R23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="S23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="T23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="U23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="V23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="X23" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y23" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="CS23">
         <v>1</v>
@@ -4951,45 +4960,45 @@
         <v>24</v>
       </c>
       <c r="DW23" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX23" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY23" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="24" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="B24" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C24">
         <v>1</v>
       </c>
       <c r="D24" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E24" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F24" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="G24" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J24">
         <v>16</v>
       </c>
       <c r="K24" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L24">
         <v>12</v>
@@ -4998,16 +5007,16 @@
         <v>2</v>
       </c>
       <c r="V24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="X24" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y24" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="CS24" s="6">
         <v>6</v>
@@ -5016,45 +5025,45 @@
         <v>15</v>
       </c>
       <c r="DW24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX24" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY24" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="25" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
-        <v>244</v>
+        <v>242</v>
       </c>
       <c r="B25" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C25">
         <v>0</v>
       </c>
       <c r="D25" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E25" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="F25" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="G25" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J25">
         <v>16</v>
       </c>
       <c r="K25" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L25">
         <v>12</v>
@@ -5063,16 +5072,16 @@
         <v>2</v>
       </c>
       <c r="V25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="X25" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y25" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="CS25" s="6">
         <v>1</v>
@@ -5081,45 +5090,45 @@
         <v>13</v>
       </c>
       <c r="DW25" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="DX25" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY25" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="26" spans="1:129" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B26" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
       <c r="C26">
         <v>1</v>
       </c>
       <c r="D26" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="E26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="F26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="G26" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="I26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="J26">
         <v>16</v>
       </c>
       <c r="K26" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
       <c r="L26">
         <v>12</v>
@@ -5128,16 +5137,16 @@
         <v>2</v>
       </c>
       <c r="V26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="W26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="X26" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="Y26" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="CS26" s="6">
         <v>2</v>
@@ -5146,13 +5155,13 @@
         <v>14</v>
       </c>
       <c r="DW26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="DX26" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="DY26" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Minor corrections of mistakes, revisions
Corrected few data in the dataset (e.g., adding data for sedation in Tsukada et al 2023, and insominia in Isaacson et al 2023)
</commit_message>
<xml_diff>
--- a/data/LSR3_H_2024-01-22.xlsx
+++ b/data/LSR3_H_2024-01-22.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sksiafis/Documents/GitHub/LSR3_taar1_H/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FA813AA-6DB1-A44A-8916-E1F1BF25456C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB4DC28F-7A56-AB48-87B9-A39D92320524}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-24460" yWindow="-21100" windowWidth="38400" windowHeight="21100" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24460" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -790,7 +790,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -821,6 +821,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -834,7 +846,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -847,6 +859,8 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1153,8 +1167,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:DY26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="CD1" workbookViewId="0">
-      <selection activeCell="CS10" sqref="CS10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="CR19" sqref="A19:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1716,6 +1730,8 @@
       <c r="CT2">
         <v>25</v>
       </c>
+      <c r="CW2" s="9"/>
+      <c r="CX2" s="9"/>
       <c r="CY2">
         <v>4</v>
       </c>
@@ -1734,11 +1750,16 @@
       <c r="DF2">
         <v>25</v>
       </c>
+      <c r="DK2" s="9"/>
+      <c r="DL2" s="9"/>
       <c r="DM2">
         <v>13</v>
       </c>
       <c r="DN2">
         <v>25</v>
+      </c>
+      <c r="DO2" s="8">
+        <v>2</v>
       </c>
       <c r="DW2" t="s">
         <v>139</v>
@@ -4357,7 +4378,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="18" spans="1:129" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:129" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>224</v>
       </c>
@@ -4544,6 +4565,12 @@
         <v>1</v>
       </c>
       <c r="DD19">
+        <v>63</v>
+      </c>
+      <c r="DE19" s="8">
+        <v>0</v>
+      </c>
+      <c r="DF19">
         <v>63</v>
       </c>
       <c r="DI19">

</xml_diff>